<commit_message>
data provider code reading from excel file
</commit_message>
<xml_diff>
--- a/PageFactoryFw/src/main/java/com/framework/automation/PageFactoryFw/data/TestData.xlsx
+++ b/PageFactoryFw/src/main/java/com/framework/automation/PageFactoryFw/data/TestData.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="19320" windowHeight="6330"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16815" windowHeight="6330"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginData" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:S19"/>
+  <oleSize ref="A1:L19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Username</t>
   </si>
@@ -26,13 +26,25 @@
   </si>
   <si>
     <t>Runmode</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>pass123</t>
+  </si>
+  <si>
+    <t>test1@gmail.com</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -47,6 +59,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,14 +85,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -366,15 +391,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -389,9 +414,35 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
code for capturing screenshots and linking screenshots to testng reports
</commit_message>
<xml_diff>
--- a/PageFactoryFw/src/main/java/com/framework/automation/PageFactoryFw/data/TestData.xlsx
+++ b/PageFactoryFw/src/main/java/com/framework/automation/PageFactoryFw/data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="16815" windowHeight="6330"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14310" windowHeight="6330"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Username</t>
   </si>
@@ -38,6 +38,21 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>test3@yahoo.com</t>
+  </si>
+  <si>
+    <t>pass2322</t>
+  </si>
+  <si>
+    <t>test4@hotmail.com</t>
+  </si>
+  <si>
+    <t>pass121</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -391,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -436,13 +451,37 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>